<commit_message>
Exercise 2 Part 2
Cleaned data in exampledata2 and saved as processeddata2. Created boxplot and scatterplot as specified in the instructions with the new variables and saved them to figures folder.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3330FBB3-0F10-47E2-8811-7A4CCD163C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="1177" yWindow="1635" windowWidth="14400" windowHeight="8183" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Height</t>
   </si>
@@ -92,12 +93,15 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>BenchPress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,19 +421,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,13 +444,13 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>180</v>
       </c>
@@ -463,7 +467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>175</v>
       </c>
@@ -480,7 +484,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -497,7 +501,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>178</v>
       </c>
@@ -514,7 +518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>192</v>
       </c>
@@ -531,7 +535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -548,7 +552,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>156</v>
       </c>
@@ -565,7 +569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>166</v>
       </c>
@@ -582,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>155</v>
       </c>
@@ -599,7 +603,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>145</v>
       </c>
@@ -616,7 +620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>165</v>
       </c>
@@ -630,7 +634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>133</v>
       </c>
@@ -647,7 +651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>166</v>
       </c>
@@ -664,7 +668,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>154</v>
       </c>
@@ -687,21 +691,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -712,7 +716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -723,7 +727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -734,7 +738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -745,7 +749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -756,7 +760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>18</v>
       </c>

</xml_diff>